<commit_message>
Added case where pool was smaller than required
</commit_message>
<xml_diff>
--- a/frontierResults.xlsx
+++ b/frontierResults.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmccall/Documents/omega_h-kokkos-mempool-paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB65229D-4537-6549-9345-388DAC712657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96EA6E3B-8138-F948-A474-C40A1EA82711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53180" yWindow="2240" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
-    <sheet name="summarized" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="frontierResults" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
   <si>
     <t>case</t>
   </si>
@@ -47,7 +47,13 @@
     <t>reducedThrust</t>
   </si>
   <si>
+    <t>reducedPool</t>
+  </si>
+  <si>
     <t>50k</t>
+  </si>
+  <si>
+    <t>Sum of time</t>
   </si>
   <si>
     <t>Row Labels</t>
@@ -59,13 +65,13 @@
     <t>Column Labels</t>
   </si>
   <si>
-    <t>Average of time</t>
-  </si>
-  <si>
     <t>Pool Disabled</t>
   </si>
   <si>
     <t>Pool Enabled</t>
+  </si>
+  <si>
+    <t>Pool Enabled (Reduced Size)</t>
   </si>
 </sst>
 </file>
@@ -628,71 +634,11 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[frontierResults.xlsx]summarized!PivotTable2</c:name>
+    <c:name>[frontierResults.xlsx]Sheet1!PivotTable3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Delta</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Wing Case Benchmarks on Frontier</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
@@ -718,13 +664,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -774,13 +718,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="75000"/>
@@ -817,12 +759,78 @@
           </a:ln>
           <a:effectLst/>
         </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
           <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
             <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -842,7 +850,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>summarized!$B$3:$B$4</c:f>
+              <c:f>Sheet1!$B$3:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -870,13 +878,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -920,7 +926,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>summarized!$A$5:$A$7</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -934,12 +940,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>summarized!$B$5:$B$7</c:f>
+              <c:f>Sheet1!$B$5:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4.569445</c:v>
+                  <c:v>18.27778</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.89119599999999999</c:v>
@@ -949,7 +955,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9BF8-6A47-AE5B-E056A72EA02F}"/>
+              <c16:uniqueId val="{00000000-9A6A-304D-B071-AE842158136D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -958,7 +964,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>summarized!$C$3:$C$4</c:f>
+              <c:f>Sheet1!$C$3:$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -986,13 +992,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1036,7 +1040,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>summarized!$A$5:$A$7</c:f>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1050,12 +1054,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>summarized!$C$5:$C$7</c:f>
+              <c:f>Sheet1!$C$5:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2.8924837499999998</c:v>
+                  <c:v>11.569934999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.49179099999999998</c:v>
@@ -1065,7 +1069,121 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9BF8-6A47-AE5B-E056A72EA02F}"/>
+              <c16:uniqueId val="{00000001-9A6A-304D-B071-AE842158136D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pool Enabled (Reduced Size)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>500k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>11.570081999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49014000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9A6A-304D-B071-AE842158136D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1078,11 +1196,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="1076961600"/>
-        <c:axId val="1077752992"/>
+        <c:axId val="124441551"/>
+        <c:axId val="124443279"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1076961600"/>
+        <c:axId val="124441551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1228,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1125,7 +1243,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1077752992"/>
+        <c:crossAx val="124443279"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1133,7 +1251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1077752992"/>
+        <c:axId val="124443279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1264,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1160,7 +1278,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time in seconds (lower is better)</a:t>
+                  <a:t>Time (seconds) Lower is better</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1178,7 +1296,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1210,7 +1328,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1225,7 +1343,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1076961600"/>
+        <c:crossAx val="124441551"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1252,7 +1370,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1299,7 +1417,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1100"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1882,7 +2000,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:colOff>774700</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -1891,7 +2009,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C04BAAD-EC32-E650-18C0-2D418520D98C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8A10877-B32F-0358-3783-3CE1AFAB1C76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1913,9 +2031,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Matthew McCall" refreshedDate="45156.657198842593" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="10">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Matthew McCall" refreshedDate="45159.615971990737" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="15">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D11" sheet="frontierResults"/>
+    <worksheetSource ref="A1:D16" sheet="frontierResults"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="case" numFmtId="0">
@@ -1925,16 +2043,17 @@
       </sharedItems>
     </cacheField>
     <cacheField name="pool" numFmtId="0">
-      <sharedItems count="2">
+      <sharedItems count="3">
         <s v="nopool"/>
         <s v="pool"/>
+        <s v="reducedPool"/>
       </sharedItems>
     </cacheField>
     <cacheField name="branch" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.49179099999999998" maxValue="6.7944899999999997"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.49014000000000002" maxValue="6.7944899999999997"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1946,7 +2065,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="15">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -1996,6 +2115,30 @@
     <n v="3.9856699999999998"/>
   </r>
   <r>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="reducedThrust"/>
+    <n v="0.90657200000000004"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="reducedThrust"/>
+    <n v="3.3220000000000001"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="reducedThrust"/>
+    <n v="3.3582299999999998"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="reducedThrust"/>
+    <n v="3.9832800000000002"/>
+  </r>
+  <r>
     <x v="1"/>
     <x v="0"/>
     <s v="reducedThrust"/>
@@ -2007,12 +2150,18 @@
     <s v="reducedThrust"/>
     <n v="0.49179099999999998"/>
   </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="reducedThrust"/>
+    <n v="0.49014000000000002"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
@@ -2022,9 +2171,10 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="3">
+      <items count="4">
         <item n="Pool Disabled" x="0"/>
         <item n="Pool Enabled" x="1"/>
+        <item n="Pool Enabled (Reduced Size)" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2048,21 +2198,24 @@
   <colFields count="1">
     <field x="1"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
+    <i>
+      <x v="2"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of time" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Sum of time" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="4">
+  <chartFormats count="6">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -2087,7 +2240,19 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="2">
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -2102,7 +2267,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="3">
+    <chartFormat chart="0" format="4">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -2113,6 +2278,21 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -2427,59 +2607,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D7"/>
+  <dimension ref="A3:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4.569445</v>
+        <v>18.27778</v>
       </c>
       <c r="C5" s="1">
-        <v>2.8924837499999998</v>
+        <v>11.569934999999999</v>
       </c>
       <c r="D5" s="1">
-        <v>3.7309643750000001</v>
+        <v>11.570081999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>41.417797</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>0.89119599999999999</v>
@@ -2488,21 +2674,27 @@
         <v>0.49179099999999998</v>
       </c>
       <c r="D6" s="1">
-        <v>0.69149349999999998</v>
+        <v>0.49014000000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.873127</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>3.8337952</v>
+        <v>19.168976000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>2.4123451999999999</v>
+        <v>12.061725999999998</v>
       </c>
       <c r="D7" s="1">
-        <v>3.1230701999999999</v>
+        <v>12.060222</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43.290923999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2513,13 +2705,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:D11"/>
+      <selection sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2649,30 +2844,100 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
         <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10">
-        <v>0.89119599999999999</v>
+        <v>0.90657200000000004</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
+        <v>3.3220000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>3.3582299999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>3.9832800000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>0.89119599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
         <v>0.49179099999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>0.49014000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>